<commit_message>
feat: added relationships between tables in the models
</commit_message>
<xml_diff>
--- a/relaciones tablas/estructura de tablas.xlsx
+++ b/relaciones tablas/estructura de tablas.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="44">
   <si>
     <t xml:space="preserve">Tattoo Store</t>
   </si>
@@ -39,7 +39,7 @@
     <t xml:space="preserve">roles</t>
   </si>
   <si>
-    <t xml:space="preserve">user_role</t>
+    <t xml:space="preserve">role_user</t>
   </si>
   <si>
     <t xml:space="preserve">worker</t>
@@ -75,76 +75,82 @@
     <t xml:space="preserve">email </t>
   </si>
   <si>
+    <t xml:space="preserve">privilege</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hours_worked</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">created_at</t>
+  </si>
+  <si>
+    <t xml:space="preserve">timestamp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phone_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">updated_at</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is_Active</t>
+  </si>
+  <si>
+    <t xml:space="preserve">boolean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clients</t>
+  </si>
+  <si>
+    <t xml:space="preserve">appointments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">portfolio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">portfolio_worker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">client_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">portfolio_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">worker_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">float</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">time</t>
+  </si>
+  <si>
     <t xml:space="preserve">description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hours_worked</t>
-  </si>
-  <si>
-    <t xml:space="preserve">password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">created_at</t>
-  </si>
-  <si>
-    <t xml:space="preserve">timestamp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phone_number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">updated_at</t>
-  </si>
-  <si>
-    <t xml:space="preserve">is_Active</t>
-  </si>
-  <si>
-    <t xml:space="preserve">boolean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">clients</t>
-  </si>
-  <si>
-    <t xml:space="preserve">appointments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">portfolio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">portfolio_worker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">client_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">name </t>
-  </si>
-  <si>
-    <t xml:space="preserve">portfolio_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">worker_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">image</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hour</t>
-  </si>
-  <si>
-    <t xml:space="preserve">time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">float</t>
   </si>
   <si>
     <t xml:space="preserve">*ver si la fecha es anterior al día </t>
@@ -389,7 +395,7 @@
   <dimension ref="B1:L1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+      <selection pane="topLeft" activeCell="J21" activeCellId="0" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -401,7 +407,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="10.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="10.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="10.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -718,13 +726,13 @@
         <v>35</v>
       </c>
       <c r="F18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="I18" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="K18" s="3" t="s">
         <v>21</v>
@@ -735,10 +743,10 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E19" s="3" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>18</v>
@@ -749,7 +757,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E20" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>19</v>
@@ -758,6 +766,14 @@
         <v>21</v>
       </c>
       <c r="I20" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -802,9 +818,9 @@
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="14.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="14.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="14.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="10.54"/>
   </cols>
   <sheetData>
@@ -1027,7 +1043,7 @@
         <v>10</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>18</v>
@@ -1126,7 +1142,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D19" s="7" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1427,7 +1443,7 @@
         <v>33</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>18</v>
@@ -1450,7 +1466,7 @@
         <v>33</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>19</v>
@@ -1515,17 +1531,17 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1573,7 +1589,7 @@
         <v>34</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>18</v>
@@ -1596,7 +1612,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>19</v>

</xml_diff>